<commit_message>
Update CDEs (Copy-Paste Fehler bei Codierung behoben), neue Informationen unter "Detaillierte Spezifikationen"
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-age.xlsx
+++ b/output/StructureDefinition-cde-age.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$130</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5083" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="664">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-03T18:31:25+01:00</t>
+    <t>2023-03-04T00:41:34+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1148,59 +1148,28 @@
     <t>Observation.code.coding</t>
   </si>
   <si>
-    <t>value:code}
-value:system}</t>
-  </si>
-  <si>
-    <t>Observation.code.coding:ageCode</t>
-  </si>
-  <si>
-    <t>ageCode</t>
-  </si>
-  <si>
-    <t>Observation.code.coding:ageCode.id</t>
-  </si>
-  <si>
     <t>Observation.code.coding.id</t>
   </si>
   <si>
-    <t>Observation.code.coding:ageCode.extension</t>
-  </si>
-  <si>
     <t>Observation.code.coding.extension</t>
   </si>
   <si>
-    <t>Observation.code.coding:ageCode.system</t>
-  </si>
-  <si>
     <t>Observation.code.coding.system</t>
   </si>
   <si>
     <t>http://loinc.org</t>
   </si>
   <si>
-    <t>Observation.code.coding:ageCode.version</t>
-  </si>
-  <si>
     <t>Observation.code.coding.version</t>
   </si>
   <si>
-    <t>Observation.code.coding:ageCode.code</t>
-  </si>
-  <si>
     <t>Observation.code.coding.code</t>
   </si>
   <si>
     <t>30525-0</t>
   </si>
   <si>
-    <t>Observation.code.coding:ageCode.display</t>
-  </si>
-  <si>
     <t>Observation.code.coding.display</t>
-  </si>
-  <si>
-    <t>Observation.code.coding:ageCode.userSelected</t>
   </si>
   <si>
     <t>Observation.code.coding.userSelected</t>
@@ -2427,7 +2396,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP131"/>
+  <dimension ref="A1:AP130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -11572,7 +11541,7 @@
         <v>92</v>
       </c>
       <c r="H76" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I76" t="s" s="2">
         <v>82</v>
@@ -11654,7 +11623,7 @@
         <v>104</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="AK76" t="s" s="2">
         <v>358</v>
@@ -11932,7 +11901,7 @@
         <v>81</v>
       </c>
       <c r="H79" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I79" t="s" s="2">
         <v>82</v>
@@ -11990,14 +11959,16 @@
         <v>82</v>
       </c>
       <c r="AB79" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="AC79" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="AC79" t="s" s="2">
+        <v>82</v>
+      </c>
       <c r="AD79" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>230</v>
@@ -12035,48 +12006,42 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="C80" t="s" s="2">
-        <v>369</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
         <v>82</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G80" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H80" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I80" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O80" t="s" s="2">
-        <v>229</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
       <c r="P80" t="s" s="2">
         <v>82</v>
       </c>
@@ -12124,19 +12089,19 @@
         <v>82</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH80" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>82</v>
@@ -12145,10 +12110,10 @@
         <v>82</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>231</v>
+        <v>82</v>
       </c>
       <c r="AN80" t="s" s="2">
-        <v>232</v>
+        <v>113</v>
       </c>
       <c r="AO80" t="s" s="2">
         <v>82</v>
@@ -12159,21 +12124,21 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>82</v>
@@ -12185,15 +12150,17 @@
         <v>82</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>216</v>
+        <v>141</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N81" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>143</v>
+      </c>
       <c r="O81" s="2"/>
       <c r="P81" t="s" s="2">
         <v>82</v>
@@ -12230,31 +12197,31 @@
         <v>82</v>
       </c>
       <c r="AB81" t="s" s="2">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AC81" t="s" s="2">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD81" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>82</v>
@@ -12266,7 +12233,7 @@
         <v>82</v>
       </c>
       <c r="AN81" t="s" s="2">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="AO81" t="s" s="2">
         <v>82</v>
@@ -12277,21 +12244,21 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H82" t="s" s="2">
         <v>82</v>
@@ -12300,27 +12267,29 @@
         <v>82</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="N82" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="O82" s="2"/>
+        <v>241</v>
+      </c>
+      <c r="O82" t="s" s="2">
+        <v>242</v>
+      </c>
       <c r="P82" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q82" s="2"/>
       <c r="R82" t="s" s="2">
-        <v>82</v>
+        <v>370</v>
       </c>
       <c r="S82" t="s" s="2">
         <v>82</v>
@@ -12350,31 +12319,31 @@
         <v>82</v>
       </c>
       <c r="AB82" t="s" s="2">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="AC82" t="s" s="2">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="AD82" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI82" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="AK82" t="s" s="2">
         <v>82</v>
@@ -12383,10 +12352,10 @@
         <v>82</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>82</v>
+        <v>245</v>
       </c>
       <c r="AN82" t="s" s="2">
-        <v>106</v>
+        <v>246</v>
       </c>
       <c r="AO82" t="s" s="2">
         <v>82</v>
@@ -12397,10 +12366,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -12408,7 +12377,7 @@
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G83" t="s" s="2">
         <v>92</v>
@@ -12423,26 +12392,24 @@
         <v>93</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>108</v>
+        <v>215</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="O83" t="s" s="2">
-        <v>242</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q83" s="2"/>
       <c r="R83" t="s" s="2">
-        <v>376</v>
+        <v>82</v>
       </c>
       <c r="S83" t="s" s="2">
         <v>82</v>
@@ -12484,7 +12451,7 @@
         <v>82</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>80</v>
@@ -12505,10 +12472,10 @@
         <v>82</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="AO83" t="s" s="2">
         <v>82</v>
@@ -12519,10 +12486,10 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -12530,7 +12497,7 @@
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G84" t="s" s="2">
         <v>92</v>
@@ -12545,24 +12512,26 @@
         <v>93</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="O84" s="2"/>
+        <v>259</v>
+      </c>
+      <c r="O84" t="s" s="2">
+        <v>260</v>
+      </c>
       <c r="P84" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q84" s="2"/>
       <c r="R84" t="s" s="2">
-        <v>82</v>
+        <v>373</v>
       </c>
       <c r="S84" t="s" s="2">
         <v>82</v>
@@ -12604,7 +12573,7 @@
         <v>82</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>80</v>
@@ -12625,10 +12594,10 @@
         <v>82</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="AN84" t="s" s="2">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="AO84" t="s" s="2">
         <v>82</v>
@@ -12639,10 +12608,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12650,7 +12619,7 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G85" t="s" s="2">
         <v>92</v>
@@ -12665,26 +12634,26 @@
         <v>93</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>115</v>
+        <v>215</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="N85" t="s" s="2">
         <v>259</v>
       </c>
       <c r="O85" t="s" s="2">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="P85" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q85" s="2"/>
       <c r="R85" t="s" s="2">
-        <v>381</v>
+        <v>82</v>
       </c>
       <c r="S85" t="s" s="2">
         <v>82</v>
@@ -12726,7 +12695,7 @@
         <v>82</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>80</v>
@@ -12747,10 +12716,10 @@
         <v>82</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="AN85" t="s" s="2">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="AO85" t="s" s="2">
         <v>82</v>
@@ -12761,10 +12730,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12787,19 +12756,19 @@
         <v>93</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>215</v>
+        <v>275</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="N86" t="s" s="2">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="O86" t="s" s="2">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="P86" t="s" s="2">
         <v>82</v>
@@ -12848,7 +12817,7 @@
         <v>82</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>80</v>
@@ -12869,10 +12838,10 @@
         <v>82</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>82</v>
@@ -12883,10 +12852,10 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12894,13 +12863,13 @@
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G87" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H87" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I87" t="s" s="2">
         <v>82</v>
@@ -12909,19 +12878,19 @@
         <v>93</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>275</v>
+        <v>215</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="O87" t="s" s="2">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="P87" t="s" s="2">
         <v>82</v>
@@ -12931,7 +12900,7 @@
         <v>82</v>
       </c>
       <c r="S87" t="s" s="2">
-        <v>82</v>
+        <v>336</v>
       </c>
       <c r="T87" t="s" s="2">
         <v>82</v>
@@ -12970,7 +12939,7 @@
         <v>82</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>80</v>
@@ -12991,10 +12960,10 @@
         <v>82</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>82</v>
@@ -13005,10 +12974,10 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -13016,13 +12985,13 @@
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G88" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H88" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I88" t="s" s="2">
         <v>82</v>
@@ -13031,19 +13000,19 @@
         <v>93</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>215</v>
+        <v>378</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>285</v>
+        <v>379</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>286</v>
+        <v>380</v>
       </c>
       <c r="N88" t="s" s="2">
-        <v>287</v>
+        <v>381</v>
       </c>
       <c r="O88" t="s" s="2">
-        <v>288</v>
+        <v>382</v>
       </c>
       <c r="P88" t="s" s="2">
         <v>82</v>
@@ -13092,7 +13061,7 @@
         <v>82</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>289</v>
+        <v>377</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>80</v>
@@ -13104,22 +13073,22 @@
         <v>104</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>82</v>
+        <v>383</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>290</v>
+        <v>384</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>291</v>
+        <v>385</v>
       </c>
       <c r="AO88" t="s" s="2">
-        <v>82</v>
+        <v>386</v>
       </c>
       <c r="AP88" t="s" s="2">
         <v>82</v>
@@ -13138,13 +13107,13 @@
       </c>
       <c r="E89" s="2"/>
       <c r="F89" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G89" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H89" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I89" t="s" s="2">
         <v>82</v>
@@ -13164,9 +13133,7 @@
       <c r="N89" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="O89" t="s" s="2">
-        <v>392</v>
-      </c>
+      <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
         <v>82</v>
       </c>
@@ -13220,7 +13187,7 @@
         <v>80</v>
       </c>
       <c r="AH89" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI89" t="s" s="2">
         <v>104</v>
@@ -13229,19 +13196,19 @@
         <v>170</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>393</v>
+        <v>82</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>394</v>
+        <v>360</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="AO89" t="s" s="2">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="AP89" t="s" s="2">
         <v>82</v>
@@ -13249,21 +13216,21 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
-        <v>82</v>
+        <v>394</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G90" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H90" t="s" s="2">
         <v>82</v>
@@ -13275,18 +13242,20 @@
         <v>93</v>
       </c>
       <c r="K90" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="L90" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="M90" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="N90" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="L90" t="s" s="2">
+      <c r="O90" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="M90" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="N90" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="O90" s="2"/>
       <c r="P90" t="s" s="2">
         <v>82</v>
       </c>
@@ -13334,13 +13303,13 @@
         <v>82</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>104</v>
@@ -13349,19 +13318,19 @@
         <v>170</v>
       </c>
       <c r="AK90" t="s" s="2">
-        <v>82</v>
+        <v>400</v>
       </c>
       <c r="AL90" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>360</v>
+        <v>401</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>402</v>
       </c>
       <c r="AO90" t="s" s="2">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="AP90" t="s" s="2">
         <v>82</v>
@@ -13369,14 +13338,14 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" t="s" s="2">
@@ -13395,19 +13364,19 @@
         <v>93</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="N91" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="O91" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="P91" t="s" s="2">
         <v>82</v>
@@ -13456,7 +13425,7 @@
         <v>82</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>80</v>
@@ -13468,22 +13437,22 @@
         <v>104</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="AK91" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AL91" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AN91" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AO91" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="AP91" t="s" s="2">
         <v>82</v>
@@ -13491,14 +13460,14 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
-        <v>415</v>
+        <v>82</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" t="s" s="2">
@@ -13528,9 +13497,7 @@
       <c r="N92" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="O92" t="s" s="2">
-        <v>420</v>
-      </c>
+      <c r="O92" s="2"/>
       <c r="P92" t="s" s="2">
         <v>82</v>
       </c>
@@ -13578,7 +13545,7 @@
         <v>82</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>80</v>
@@ -13593,19 +13560,19 @@
         <v>105</v>
       </c>
       <c r="AK92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL92" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM92" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="AN92" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="AL92" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AM92" t="s" s="2">
+      <c r="AO92" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="AN92" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="AO92" t="s" s="2">
-        <v>424</v>
       </c>
       <c r="AP92" t="s" s="2">
         <v>82</v>
@@ -13613,10 +13580,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -13627,7 +13594,7 @@
         <v>80</v>
       </c>
       <c r="G93" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H93" t="s" s="2">
         <v>82</v>
@@ -13639,18 +13606,20 @@
         <v>93</v>
       </c>
       <c r="K93" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="L93" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="M93" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="L93" t="s" s="2">
+      <c r="N93" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="O93" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="M93" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="N93" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="O93" s="2"/>
       <c r="P93" t="s" s="2">
         <v>82</v>
       </c>
@@ -13698,34 +13667,34 @@
         <v>82</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH93" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI93" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ93" t="s" s="2">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="AK93" t="s" s="2">
-        <v>82</v>
+        <v>428</v>
       </c>
       <c r="AL93" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AM93" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="AN93" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="AN93" t="s" s="2">
+      <c r="AO93" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="AO93" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="AP93" t="s" s="2">
         <v>82</v>
@@ -13733,10 +13702,10 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
@@ -13747,7 +13716,7 @@
         <v>80</v>
       </c>
       <c r="G94" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H94" t="s" s="2">
         <v>82</v>
@@ -13759,16 +13728,16 @@
         <v>93</v>
       </c>
       <c r="K94" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="L94" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L94" t="s" s="2">
+      <c r="M94" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="M94" t="s" s="2">
+      <c r="N94" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="N94" t="s" s="2">
-        <v>168</v>
       </c>
       <c r="O94" t="s" s="2">
         <v>437</v>
@@ -13808,59 +13777,59 @@
         <v>82</v>
       </c>
       <c r="AB94" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC94" t="s" s="2">
-        <v>82</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="AC94" s="2"/>
       <c r="AD94" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF94" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AG94" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH94" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI94" t="s" s="2">
-        <v>104</v>
+        <v>439</v>
       </c>
       <c r="AJ94" t="s" s="2">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="AK94" t="s" s="2">
-        <v>438</v>
+        <v>82</v>
       </c>
       <c r="AL94" t="s" s="2">
-        <v>82</v>
+        <v>440</v>
       </c>
       <c r="AM94" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="AN94" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AO94" t="s" s="2">
-        <v>441</v>
+        <v>82</v>
       </c>
       <c r="AP94" t="s" s="2">
-        <v>82</v>
+        <v>443</v>
       </c>
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="C95" s="2"/>
+        <v>432</v>
+      </c>
+      <c r="C95" t="s" s="2">
+        <v>445</v>
+      </c>
       <c r="D95" t="s" s="2">
         <v>82</v>
       </c>
@@ -13881,19 +13850,19 @@
         <v>93</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="M95" t="s" s="2">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="N95" t="s" s="2">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="O95" t="s" s="2">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="P95" t="s" s="2">
         <v>82</v>
@@ -13930,59 +13899,59 @@
         <v>82</v>
       </c>
       <c r="AB95" t="s" s="2">
-        <v>448</v>
-      </c>
-      <c r="AC95" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>82</v>
+      </c>
       <c r="AD95" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF95" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="AN95" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="AG95" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH95" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="AI95" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="AJ95" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="AK95" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL95" t="s" s="2">
-        <v>450</v>
-      </c>
-      <c r="AM95" t="s" s="2">
-        <v>451</v>
-      </c>
-      <c r="AN95" t="s" s="2">
-        <v>452</v>
-      </c>
       <c r="AO95" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP95" t="s" s="2">
-        <v>453</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="C96" t="s" s="2">
-        <v>455</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
         <v>82</v>
       </c>
@@ -14000,23 +13969,19 @@
         <v>82</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>456</v>
+        <v>215</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>444</v>
+        <v>216</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>446</v>
-      </c>
-      <c r="O96" t="s" s="2">
-        <v>447</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
       <c r="P96" t="s" s="2">
         <v>82</v>
       </c>
@@ -14064,7 +14029,7 @@
         <v>82</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>442</v>
+        <v>218</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>80</v>
@@ -14073,7 +14038,7 @@
         <v>92</v>
       </c>
       <c r="AI96" t="s" s="2">
-        <v>449</v>
+        <v>82</v>
       </c>
       <c r="AJ96" t="s" s="2">
         <v>82</v>
@@ -14082,38 +14047,38 @@
         <v>82</v>
       </c>
       <c r="AL96" t="s" s="2">
-        <v>450</v>
+        <v>82</v>
       </c>
       <c r="AM96" t="s" s="2">
-        <v>451</v>
+        <v>82</v>
       </c>
       <c r="AN96" t="s" s="2">
-        <v>452</v>
+        <v>113</v>
       </c>
       <c r="AO96" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP96" t="s" s="2">
-        <v>453</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" t="s" s="2">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G97" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H97" t="s" s="2">
         <v>82</v>
@@ -14125,15 +14090,17 @@
         <v>82</v>
       </c>
       <c r="K97" t="s" s="2">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>216</v>
+        <v>141</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N97" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="N97" t="s" s="2">
+        <v>143</v>
+      </c>
       <c r="O97" s="2"/>
       <c r="P97" t="s" s="2">
         <v>82</v>
@@ -14170,31 +14137,31 @@
         <v>82</v>
       </c>
       <c r="AB97" t="s" s="2">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AC97" t="s" s="2">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD97" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE97" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH97" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI97" t="s" s="2">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AJ97" t="s" s="2">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="AK97" t="s" s="2">
         <v>82</v>
@@ -14206,7 +14173,7 @@
         <v>82</v>
       </c>
       <c r="AN97" t="s" s="2">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="AO97" t="s" s="2">
         <v>82</v>
@@ -14217,44 +14184,46 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G98" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H98" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I98" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J98" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K98" t="s" s="2">
-        <v>140</v>
+        <v>453</v>
       </c>
       <c r="L98" t="s" s="2">
-        <v>141</v>
+        <v>454</v>
       </c>
       <c r="M98" t="s" s="2">
-        <v>221</v>
+        <v>455</v>
       </c>
       <c r="N98" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="O98" s="2"/>
+        <v>456</v>
+      </c>
+      <c r="O98" t="s" s="2">
+        <v>457</v>
+      </c>
       <c r="P98" t="s" s="2">
         <v>82</v>
       </c>
@@ -14290,31 +14259,31 @@
         <v>82</v>
       </c>
       <c r="AB98" t="s" s="2">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="AC98" t="s" s="2">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="AD98" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE98" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF98" t="s" s="2">
-        <v>222</v>
+        <v>458</v>
       </c>
       <c r="AG98" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH98" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI98" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ98" t="s" s="2">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="AK98" t="s" s="2">
         <v>82</v>
@@ -14323,10 +14292,10 @@
         <v>82</v>
       </c>
       <c r="AM98" t="s" s="2">
-        <v>82</v>
+        <v>459</v>
       </c>
       <c r="AN98" t="s" s="2">
-        <v>106</v>
+        <v>460</v>
       </c>
       <c r="AO98" t="s" s="2">
         <v>82</v>
@@ -14348,65 +14317,67 @@
       </c>
       <c r="E99" s="2"/>
       <c r="F99" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G99" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="I99" t="s" s="2">
         <v>93</v>
-      </c>
-      <c r="I99" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="J99" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K99" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="L99" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="L99" t="s" s="2">
+      <c r="M99" t="s" s="2">
         <v>464</v>
       </c>
-      <c r="M99" t="s" s="2">
+      <c r="N99" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="O99" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="N99" t="s" s="2">
+      <c r="P99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Q99" t="s" s="2">
         <v>466</v>
       </c>
-      <c r="O99" t="s" s="2">
+      <c r="R99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W99" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X99" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="Y99" t="s" s="2">
         <v>467</v>
       </c>
-      <c r="P99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Q99" s="2"/>
-      <c r="R99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="S99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Y99" t="s" s="2">
-        <v>82</v>
-      </c>
       <c r="Z99" t="s" s="2">
-        <v>82</v>
+        <v>468</v>
       </c>
       <c r="AA99" t="s" s="2">
         <v>82</v>
@@ -14424,7 +14395,7 @@
         <v>82</v>
       </c>
       <c r="AF99" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AG99" t="s" s="2">
         <v>80</v>
@@ -14445,10 +14416,10 @@
         <v>82</v>
       </c>
       <c r="AM99" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AN99" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AO99" t="s" s="2">
         <v>82</v>
@@ -14459,10 +14430,10 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -14470,41 +14441,39 @@
       </c>
       <c r="E100" s="2"/>
       <c r="F100" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G100" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H100" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I100" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J100" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>115</v>
+        <v>215</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="N100" t="s" s="2">
         <v>259</v>
       </c>
       <c r="O100" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="P100" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="Q100" t="s" s="2">
-        <v>476</v>
-      </c>
+      <c r="Q100" s="2"/>
       <c r="R100" t="s" s="2">
         <v>82</v>
       </c>
@@ -14524,31 +14493,31 @@
         <v>82</v>
       </c>
       <c r="X100" t="s" s="2">
-        <v>188</v>
+        <v>82</v>
       </c>
       <c r="Y100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="Z100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AA100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AB100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AC100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AD100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AE100" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AF100" t="s" s="2">
         <v>477</v>
-      </c>
-      <c r="Z100" t="s" s="2">
-        <v>478</v>
-      </c>
-      <c r="AA100" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AB100" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC100" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AD100" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AE100" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF100" t="s" s="2">
-        <v>479</v>
       </c>
       <c r="AG100" t="s" s="2">
         <v>80</v>
@@ -14569,10 +14538,10 @@
         <v>82</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="AN100" t="s" s="2">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="AO100" t="s" s="2">
         <v>82</v>
@@ -14583,10 +14552,10 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
@@ -14609,26 +14578,26 @@
         <v>93</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>215</v>
+        <v>108</v>
       </c>
       <c r="L101" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="M101" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="N101" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="M101" t="s" s="2">
+      <c r="O101" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="N101" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="O101" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="P101" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q101" s="2"/>
       <c r="R101" t="s" s="2">
-        <v>82</v>
+        <v>486</v>
       </c>
       <c r="S101" t="s" s="2">
         <v>82</v>
@@ -14679,7 +14648,7 @@
         <v>92</v>
       </c>
       <c r="AI101" t="s" s="2">
-        <v>104</v>
+        <v>488</v>
       </c>
       <c r="AJ101" t="s" s="2">
         <v>105</v>
@@ -14691,7 +14660,7 @@
         <v>82</v>
       </c>
       <c r="AM101" t="s" s="2">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="AN101" t="s" s="2">
         <v>489</v>
@@ -14731,50 +14700,50 @@
         <v>93</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L102" t="s" s="2">
         <v>492</v>
       </c>
       <c r="M102" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="N102" t="s" s="2">
         <v>493</v>
       </c>
-      <c r="N102" t="s" s="2">
+      <c r="O102" t="s" s="2">
         <v>494</v>
-      </c>
-      <c r="O102" t="s" s="2">
-        <v>495</v>
       </c>
       <c r="P102" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q102" s="2"/>
       <c r="R102" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="S102" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="T102" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="U102" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="V102" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="W102" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="X102" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="Y102" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="Z102" t="s" s="2">
         <v>496</v>
-      </c>
-      <c r="S102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Y102" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Z102" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="AA102" t="s" s="2">
         <v>82</v>
@@ -14801,7 +14770,7 @@
         <v>92</v>
       </c>
       <c r="AI102" t="s" s="2">
-        <v>498</v>
+        <v>104</v>
       </c>
       <c r="AJ102" t="s" s="2">
         <v>105</v>
@@ -14813,10 +14782,10 @@
         <v>82</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="AN102" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AO102" t="s" s="2">
         <v>82</v>
@@ -14827,10 +14796,10 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14838,34 +14807,34 @@
       </c>
       <c r="E103" s="2"/>
       <c r="F103" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G103" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H103" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I103" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>115</v>
+        <v>198</v>
       </c>
       <c r="L103" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="M103" t="s" s="2">
+        <v>501</v>
+      </c>
+      <c r="N103" t="s" s="2">
         <v>502</v>
       </c>
-      <c r="M103" t="s" s="2">
-        <v>502</v>
-      </c>
-      <c r="N103" t="s" s="2">
+      <c r="O103" t="s" s="2">
         <v>503</v>
-      </c>
-      <c r="O103" t="s" s="2">
-        <v>504</v>
       </c>
       <c r="P103" t="s" s="2">
         <v>82</v>
@@ -14890,7 +14859,7 @@
         <v>82</v>
       </c>
       <c r="X103" t="s" s="2">
-        <v>188</v>
+        <v>504</v>
       </c>
       <c r="Y103" t="s" s="2">
         <v>505</v>
@@ -14914,16 +14883,16 @@
         <v>82</v>
       </c>
       <c r="AF103" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="AG103" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AH103" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="AI103" t="s" s="2">
         <v>507</v>
-      </c>
-      <c r="AG103" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH103" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="AI103" t="s" s="2">
-        <v>104</v>
       </c>
       <c r="AJ103" t="s" s="2">
         <v>105</v>
@@ -14935,7 +14904,7 @@
         <v>82</v>
       </c>
       <c r="AM103" t="s" s="2">
-        <v>488</v>
+        <v>106</v>
       </c>
       <c r="AN103" t="s" s="2">
         <v>508</v>
@@ -14956,14 +14925,14 @@
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
-        <v>82</v>
+        <v>510</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G104" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H104" t="s" s="2">
         <v>82</v>
@@ -14978,16 +14947,16 @@
         <v>198</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="N104" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="O104" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P104" t="s" s="2">
         <v>82</v>
@@ -15012,7 +14981,7 @@
         <v>82</v>
       </c>
       <c r="X104" t="s" s="2">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="Y104" t="s" s="2">
         <v>515</v>
@@ -15042,10 +15011,10 @@
         <v>80</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI104" t="s" s="2">
-        <v>517</v>
+        <v>104</v>
       </c>
       <c r="AJ104" t="s" s="2">
         <v>105</v>
@@ -15054,31 +15023,31 @@
         <v>82</v>
       </c>
       <c r="AL104" t="s" s="2">
-        <v>82</v>
+        <v>517</v>
       </c>
       <c r="AM104" t="s" s="2">
-        <v>106</v>
+        <v>518</v>
       </c>
       <c r="AN104" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="AO104" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP104" t="s" s="2">
-        <v>82</v>
+        <v>520</v>
       </c>
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
-        <v>520</v>
+        <v>82</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" t="s" s="2">
@@ -15097,19 +15066,19 @@
         <v>82</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>198</v>
+        <v>522</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="M105" t="s" s="2">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="N105" t="s" s="2">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="O105" t="s" s="2">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="P105" t="s" s="2">
         <v>82</v>
@@ -15134,13 +15103,13 @@
         <v>82</v>
       </c>
       <c r="X105" t="s" s="2">
-        <v>514</v>
+        <v>82</v>
       </c>
       <c r="Y105" t="s" s="2">
-        <v>525</v>
+        <v>82</v>
       </c>
       <c r="Z105" t="s" s="2">
-        <v>526</v>
+        <v>82</v>
       </c>
       <c r="AA105" t="s" s="2">
         <v>82</v>
@@ -15158,7 +15127,7 @@
         <v>82</v>
       </c>
       <c r="AF105" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="AG105" t="s" s="2">
         <v>80</v>
@@ -15176,27 +15145,27 @@
         <v>82</v>
       </c>
       <c r="AL105" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AM105" t="s" s="2">
         <v>527</v>
       </c>
-      <c r="AM105" t="s" s="2">
+      <c r="AN105" t="s" s="2">
         <v>528</v>
       </c>
-      <c r="AN105" t="s" s="2">
-        <v>529</v>
-      </c>
       <c r="AO105" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP105" t="s" s="2">
-        <v>530</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
@@ -15207,7 +15176,7 @@
         <v>80</v>
       </c>
       <c r="G106" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H106" t="s" s="2">
         <v>82</v>
@@ -15219,20 +15188,18 @@
         <v>82</v>
       </c>
       <c r="K106" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L106" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="M106" t="s" s="2">
+        <v>531</v>
+      </c>
+      <c r="N106" t="s" s="2">
         <v>532</v>
       </c>
-      <c r="L106" t="s" s="2">
-        <v>533</v>
-      </c>
-      <c r="M106" t="s" s="2">
-        <v>534</v>
-      </c>
-      <c r="N106" t="s" s="2">
-        <v>535</v>
-      </c>
-      <c r="O106" t="s" s="2">
-        <v>536</v>
-      </c>
+      <c r="O106" s="2"/>
       <c r="P106" t="s" s="2">
         <v>82</v>
       </c>
@@ -15256,13 +15223,13 @@
         <v>82</v>
       </c>
       <c r="X106" t="s" s="2">
-        <v>82</v>
+        <v>355</v>
       </c>
       <c r="Y106" t="s" s="2">
-        <v>82</v>
+        <v>533</v>
       </c>
       <c r="Z106" t="s" s="2">
-        <v>82</v>
+        <v>534</v>
       </c>
       <c r="AA106" t="s" s="2">
         <v>82</v>
@@ -15280,13 +15247,13 @@
         <v>82</v>
       </c>
       <c r="AF106" t="s" s="2">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="AG106" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH106" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI106" t="s" s="2">
         <v>104</v>
@@ -15298,19 +15265,19 @@
         <v>82</v>
       </c>
       <c r="AL106" t="s" s="2">
-        <v>82</v>
+        <v>535</v>
       </c>
       <c r="AM106" t="s" s="2">
+        <v>536</v>
+      </c>
+      <c r="AN106" t="s" s="2">
         <v>537</v>
       </c>
-      <c r="AN106" t="s" s="2">
+      <c r="AO106" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP106" t="s" s="2">
         <v>538</v>
-      </c>
-      <c r="AO106" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP106" t="s" s="2">
-        <v>82</v>
       </c>
     </row>
     <row r="107" hidden="true">
@@ -15352,7 +15319,9 @@
       <c r="N107" t="s" s="2">
         <v>542</v>
       </c>
-      <c r="O107" s="2"/>
+      <c r="O107" t="s" s="2">
+        <v>543</v>
+      </c>
       <c r="P107" t="s" s="2">
         <v>82</v>
       </c>
@@ -15379,10 +15348,10 @@
         <v>355</v>
       </c>
       <c r="Y107" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="Z107" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AA107" t="s" s="2">
         <v>82</v>
@@ -15418,7 +15387,7 @@
         <v>82</v>
       </c>
       <c r="AL107" t="s" s="2">
-        <v>545</v>
+        <v>82</v>
       </c>
       <c r="AM107" t="s" s="2">
         <v>546</v>
@@ -15430,15 +15399,15 @@
         <v>82</v>
       </c>
       <c r="AP107" t="s" s="2">
-        <v>548</v>
+        <v>82</v>
       </c>
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -15461,7 +15430,7 @@
         <v>82</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>198</v>
+        <v>549</v>
       </c>
       <c r="L108" t="s" s="2">
         <v>550</v>
@@ -15472,9 +15441,7 @@
       <c r="N108" t="s" s="2">
         <v>552</v>
       </c>
-      <c r="O108" t="s" s="2">
-        <v>553</v>
-      </c>
+      <c r="O108" s="2"/>
       <c r="P108" t="s" s="2">
         <v>82</v>
       </c>
@@ -15498,13 +15465,13 @@
         <v>82</v>
       </c>
       <c r="X108" t="s" s="2">
-        <v>355</v>
+        <v>82</v>
       </c>
       <c r="Y108" t="s" s="2">
-        <v>554</v>
+        <v>82</v>
       </c>
       <c r="Z108" t="s" s="2">
-        <v>555</v>
+        <v>82</v>
       </c>
       <c r="AA108" t="s" s="2">
         <v>82</v>
@@ -15522,7 +15489,7 @@
         <v>82</v>
       </c>
       <c r="AF108" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>80</v>
@@ -15534,33 +15501,33 @@
         <v>104</v>
       </c>
       <c r="AJ108" t="s" s="2">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="AK108" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL108" t="s" s="2">
-        <v>82</v>
+        <v>553</v>
       </c>
       <c r="AM108" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="AN108" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="AO108" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP108" t="s" s="2">
         <v>556</v>
-      </c>
-      <c r="AN108" t="s" s="2">
-        <v>557</v>
-      </c>
-      <c r="AO108" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP108" t="s" s="2">
-        <v>82</v>
       </c>
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
@@ -15583,16 +15550,16 @@
         <v>82</v>
       </c>
       <c r="K109" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="L109" t="s" s="2">
         <v>559</v>
       </c>
-      <c r="L109" t="s" s="2">
+      <c r="M109" t="s" s="2">
         <v>560</v>
       </c>
-      <c r="M109" t="s" s="2">
+      <c r="N109" t="s" s="2">
         <v>561</v>
-      </c>
-      <c r="N109" t="s" s="2">
-        <v>562</v>
       </c>
       <c r="O109" s="2"/>
       <c r="P109" t="s" s="2">
@@ -15642,7 +15609,7 @@
         <v>82</v>
       </c>
       <c r="AF109" t="s" s="2">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>80</v>
@@ -15660,27 +15627,27 @@
         <v>82</v>
       </c>
       <c r="AL109" t="s" s="2">
+        <v>562</v>
+      </c>
+      <c r="AM109" t="s" s="2">
         <v>563</v>
       </c>
-      <c r="AM109" t="s" s="2">
+      <c r="AN109" t="s" s="2">
         <v>564</v>
       </c>
-      <c r="AN109" t="s" s="2">
+      <c r="AO109" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="AP109" t="s" s="2">
         <v>565</v>
-      </c>
-      <c r="AO109" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP109" t="s" s="2">
-        <v>566</v>
       </c>
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
@@ -15691,7 +15658,7 @@
         <v>80</v>
       </c>
       <c r="G110" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H110" t="s" s="2">
         <v>82</v>
@@ -15703,18 +15670,20 @@
         <v>82</v>
       </c>
       <c r="K110" t="s" s="2">
+        <v>567</v>
+      </c>
+      <c r="L110" t="s" s="2">
         <v>568</v>
       </c>
-      <c r="L110" t="s" s="2">
+      <c r="M110" t="s" s="2">
         <v>569</v>
       </c>
-      <c r="M110" t="s" s="2">
+      <c r="N110" t="s" s="2">
         <v>570</v>
       </c>
-      <c r="N110" t="s" s="2">
+      <c r="O110" t="s" s="2">
         <v>571</v>
       </c>
-      <c r="O110" s="2"/>
       <c r="P110" t="s" s="2">
         <v>82</v>
       </c>
@@ -15762,25 +15731,25 @@
         <v>82</v>
       </c>
       <c r="AF110" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH110" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI110" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ110" t="s" s="2">
-        <v>170</v>
+        <v>572</v>
       </c>
       <c r="AK110" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL110" t="s" s="2">
-        <v>572</v>
+        <v>82</v>
       </c>
       <c r="AM110" t="s" s="2">
         <v>573</v>
@@ -15792,15 +15761,15 @@
         <v>82</v>
       </c>
       <c r="AP110" t="s" s="2">
-        <v>575</v>
+        <v>82</v>
       </c>
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
@@ -15811,7 +15780,7 @@
         <v>80</v>
       </c>
       <c r="G111" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H111" t="s" s="2">
         <v>82</v>
@@ -15823,20 +15792,16 @@
         <v>82</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>577</v>
+        <v>215</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>578</v>
+        <v>216</v>
       </c>
       <c r="M111" t="s" s="2">
-        <v>579</v>
-      </c>
-      <c r="N111" t="s" s="2">
-        <v>580</v>
-      </c>
-      <c r="O111" t="s" s="2">
-        <v>581</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N111" s="2"/>
+      <c r="O111" s="2"/>
       <c r="P111" t="s" s="2">
         <v>82</v>
       </c>
@@ -15884,19 +15849,19 @@
         <v>82</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>576</v>
+        <v>218</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH111" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI111" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AJ111" t="s" s="2">
-        <v>582</v>
+        <v>82</v>
       </c>
       <c r="AK111" t="s" s="2">
         <v>82</v>
@@ -15905,10 +15870,10 @@
         <v>82</v>
       </c>
       <c r="AM111" t="s" s="2">
-        <v>583</v>
+        <v>82</v>
       </c>
       <c r="AN111" t="s" s="2">
-        <v>584</v>
+        <v>113</v>
       </c>
       <c r="AO111" t="s" s="2">
         <v>82</v>
@@ -15919,21 +15884,21 @@
     </row>
     <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G112" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H112" t="s" s="2">
         <v>82</v>
@@ -15945,15 +15910,17 @@
         <v>82</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>216</v>
+        <v>141</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N112" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="N112" t="s" s="2">
+        <v>143</v>
+      </c>
       <c r="O112" s="2"/>
       <c r="P112" t="s" s="2">
         <v>82</v>
@@ -15990,31 +15957,31 @@
         <v>82</v>
       </c>
       <c r="AB112" t="s" s="2">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AC112" t="s" s="2">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD112" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF112" t="s" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AG112" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH112" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI112" t="s" s="2">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AJ112" t="s" s="2">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="AK112" t="s" s="2">
         <v>82</v>
@@ -16026,7 +15993,7 @@
         <v>82</v>
       </c>
       <c r="AN112" t="s" s="2">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="AO112" t="s" s="2">
         <v>82</v>
@@ -16037,14 +16004,14 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
-        <v>139</v>
+        <v>578</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" t="s" s="2">
@@ -16057,24 +16024,26 @@
         <v>82</v>
       </c>
       <c r="I113" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K113" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>141</v>
+        <v>579</v>
       </c>
       <c r="M113" t="s" s="2">
-        <v>221</v>
+        <v>580</v>
       </c>
       <c r="N113" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="O113" s="2"/>
+      <c r="O113" t="s" s="2">
+        <v>152</v>
+      </c>
       <c r="P113" t="s" s="2">
         <v>82</v>
       </c>
@@ -16110,19 +16079,19 @@
         <v>82</v>
       </c>
       <c r="AB113" t="s" s="2">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="AC113" t="s" s="2">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="AD113" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>222</v>
+        <v>581</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>80</v>
@@ -16157,46 +16126,44 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" t="s" s="2">
-        <v>588</v>
+        <v>82</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G114" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H114" t="s" s="2">
         <v>82</v>
       </c>
       <c r="I114" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>140</v>
+        <v>583</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="M114" t="s" s="2">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="N114" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="O114" t="s" s="2">
-        <v>152</v>
-      </c>
+        <v>586</v>
+      </c>
+      <c r="O114" s="2"/>
       <c r="P114" t="s" s="2">
         <v>82</v>
       </c>
@@ -16244,19 +16211,19 @@
         <v>82</v>
       </c>
       <c r="AF114" t="s" s="2">
-        <v>591</v>
+        <v>582</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH114" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI114" t="s" s="2">
-        <v>104</v>
+        <v>587</v>
       </c>
       <c r="AJ114" t="s" s="2">
-        <v>148</v>
+        <v>588</v>
       </c>
       <c r="AK114" t="s" s="2">
         <v>82</v>
@@ -16265,10 +16232,10 @@
         <v>82</v>
       </c>
       <c r="AM114" t="s" s="2">
-        <v>82</v>
+        <v>589</v>
       </c>
       <c r="AN114" t="s" s="2">
-        <v>106</v>
+        <v>590</v>
       </c>
       <c r="AO114" t="s" s="2">
         <v>82</v>
@@ -16279,10 +16246,10 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -16305,16 +16272,16 @@
         <v>82</v>
       </c>
       <c r="K115" t="s" s="2">
+        <v>583</v>
+      </c>
+      <c r="L115" t="s" s="2">
+        <v>592</v>
+      </c>
+      <c r="M115" t="s" s="2">
         <v>593</v>
       </c>
-      <c r="L115" t="s" s="2">
-        <v>594</v>
-      </c>
-      <c r="M115" t="s" s="2">
-        <v>595</v>
-      </c>
       <c r="N115" t="s" s="2">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="O115" s="2"/>
       <c r="P115" t="s" s="2">
@@ -16364,7 +16331,7 @@
         <v>82</v>
       </c>
       <c r="AF115" t="s" s="2">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="AG115" t="s" s="2">
         <v>80</v>
@@ -16373,10 +16340,10 @@
         <v>92</v>
       </c>
       <c r="AI115" t="s" s="2">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="AJ115" t="s" s="2">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="AK115" t="s" s="2">
         <v>82</v>
@@ -16385,10 +16352,10 @@
         <v>82</v>
       </c>
       <c r="AM115" t="s" s="2">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="AN115" t="s" s="2">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="AO115" t="s" s="2">
         <v>82</v>
@@ -16399,10 +16366,10 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
@@ -16425,18 +16392,20 @@
         <v>82</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>593</v>
+        <v>198</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="M116" t="s" s="2">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="N116" t="s" s="2">
-        <v>596</v>
-      </c>
-      <c r="O116" s="2"/>
+        <v>598</v>
+      </c>
+      <c r="O116" t="s" s="2">
+        <v>599</v>
+      </c>
       <c r="P116" t="s" s="2">
         <v>82</v>
       </c>
@@ -16460,13 +16429,13 @@
         <v>82</v>
       </c>
       <c r="X116" t="s" s="2">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="Y116" t="s" s="2">
-        <v>82</v>
+        <v>600</v>
       </c>
       <c r="Z116" t="s" s="2">
-        <v>82</v>
+        <v>601</v>
       </c>
       <c r="AA116" t="s" s="2">
         <v>82</v>
@@ -16484,7 +16453,7 @@
         <v>82</v>
       </c>
       <c r="AF116" t="s" s="2">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="AG116" t="s" s="2">
         <v>80</v>
@@ -16493,22 +16462,22 @@
         <v>92</v>
       </c>
       <c r="AI116" t="s" s="2">
-        <v>597</v>
+        <v>104</v>
       </c>
       <c r="AJ116" t="s" s="2">
-        <v>598</v>
+        <v>105</v>
       </c>
       <c r="AK116" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL116" t="s" s="2">
-        <v>82</v>
+        <v>602</v>
       </c>
       <c r="AM116" t="s" s="2">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="AN116" t="s" s="2">
-        <v>604</v>
+        <v>519</v>
       </c>
       <c r="AO116" t="s" s="2">
         <v>82</v>
@@ -16519,10 +16488,10 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -16533,7 +16502,7 @@
         <v>80</v>
       </c>
       <c r="G117" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H117" t="s" s="2">
         <v>82</v>
@@ -16548,16 +16517,16 @@
         <v>198</v>
       </c>
       <c r="L117" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="M117" t="s" s="2">
         <v>606</v>
       </c>
-      <c r="M117" t="s" s="2">
+      <c r="N117" t="s" s="2">
         <v>607</v>
       </c>
-      <c r="N117" t="s" s="2">
+      <c r="O117" t="s" s="2">
         <v>608</v>
-      </c>
-      <c r="O117" t="s" s="2">
-        <v>609</v>
       </c>
       <c r="P117" t="s" s="2">
         <v>82</v>
@@ -16582,14 +16551,14 @@
         <v>82</v>
       </c>
       <c r="X117" t="s" s="2">
-        <v>119</v>
+        <v>355</v>
       </c>
       <c r="Y117" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="Z117" t="s" s="2">
         <v>610</v>
       </c>
-      <c r="Z117" t="s" s="2">
-        <v>611</v>
-      </c>
       <c r="AA117" t="s" s="2">
         <v>82</v>
       </c>
@@ -16606,13 +16575,13 @@
         <v>82</v>
       </c>
       <c r="AF117" t="s" s="2">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="AG117" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH117" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI117" t="s" s="2">
         <v>104</v>
@@ -16624,13 +16593,13 @@
         <v>82</v>
       </c>
       <c r="AL117" t="s" s="2">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="AM117" t="s" s="2">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="AN117" t="s" s="2">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="AO117" t="s" s="2">
         <v>82</v>
@@ -16641,10 +16610,10 @@
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" t="s" s="2">
@@ -16655,7 +16624,7 @@
         <v>80</v>
       </c>
       <c r="G118" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H118" t="s" s="2">
         <v>82</v>
@@ -16667,19 +16636,19 @@
         <v>82</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>198</v>
+        <v>612</v>
       </c>
       <c r="L118" t="s" s="2">
+        <v>613</v>
+      </c>
+      <c r="M118" t="s" s="2">
+        <v>614</v>
+      </c>
+      <c r="N118" t="s" s="2">
         <v>615</v>
       </c>
-      <c r="M118" t="s" s="2">
+      <c r="O118" t="s" s="2">
         <v>616</v>
-      </c>
-      <c r="N118" t="s" s="2">
-        <v>617</v>
-      </c>
-      <c r="O118" t="s" s="2">
-        <v>618</v>
       </c>
       <c r="P118" t="s" s="2">
         <v>82</v>
@@ -16704,13 +16673,13 @@
         <v>82</v>
       </c>
       <c r="X118" t="s" s="2">
-        <v>355</v>
+        <v>82</v>
       </c>
       <c r="Y118" t="s" s="2">
-        <v>619</v>
+        <v>82</v>
       </c>
       <c r="Z118" t="s" s="2">
-        <v>620</v>
+        <v>82</v>
       </c>
       <c r="AA118" t="s" s="2">
         <v>82</v>
@@ -16728,31 +16697,31 @@
         <v>82</v>
       </c>
       <c r="AF118" t="s" s="2">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="AG118" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH118" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI118" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ118" t="s" s="2">
-        <v>105</v>
+        <v>617</v>
       </c>
       <c r="AK118" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL118" t="s" s="2">
-        <v>612</v>
+        <v>82</v>
       </c>
       <c r="AM118" t="s" s="2">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="AN118" t="s" s="2">
-        <v>529</v>
+        <v>619</v>
       </c>
       <c r="AO118" t="s" s="2">
         <v>82</v>
@@ -16763,10 +16732,10 @@
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B119" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" t="s" s="2">
@@ -16789,20 +16758,18 @@
         <v>82</v>
       </c>
       <c r="K119" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="L119" t="s" s="2">
+        <v>621</v>
+      </c>
+      <c r="M119" t="s" s="2">
         <v>622</v>
       </c>
-      <c r="L119" t="s" s="2">
-        <v>623</v>
-      </c>
-      <c r="M119" t="s" s="2">
-        <v>624</v>
-      </c>
       <c r="N119" t="s" s="2">
-        <v>625</v>
-      </c>
-      <c r="O119" t="s" s="2">
-        <v>626</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="O119" s="2"/>
       <c r="P119" t="s" s="2">
         <v>82</v>
       </c>
@@ -16850,7 +16817,7 @@
         <v>82</v>
       </c>
       <c r="AF119" t="s" s="2">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AG119" t="s" s="2">
         <v>80</v>
@@ -16862,7 +16829,7 @@
         <v>104</v>
       </c>
       <c r="AJ119" t="s" s="2">
-        <v>627</v>
+        <v>105</v>
       </c>
       <c r="AK119" t="s" s="2">
         <v>82</v>
@@ -16871,10 +16838,10 @@
         <v>82</v>
       </c>
       <c r="AM119" t="s" s="2">
-        <v>628</v>
+        <v>589</v>
       </c>
       <c r="AN119" t="s" s="2">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="AO119" t="s" s="2">
         <v>82</v>
@@ -16885,10 +16852,10 @@
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
@@ -16899,7 +16866,7 @@
         <v>80</v>
       </c>
       <c r="G120" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H120" t="s" s="2">
         <v>82</v>
@@ -16908,19 +16875,19 @@
         <v>82</v>
       </c>
       <c r="J120" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K120" t="s" s="2">
-        <v>215</v>
+        <v>625</v>
       </c>
       <c r="L120" t="s" s="2">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="M120" t="s" s="2">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="N120" t="s" s="2">
-        <v>259</v>
+        <v>628</v>
       </c>
       <c r="O120" s="2"/>
       <c r="P120" t="s" s="2">
@@ -16970,19 +16937,19 @@
         <v>82</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="AG120" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH120" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI120" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ120" t="s" s="2">
-        <v>105</v>
+        <v>170</v>
       </c>
       <c r="AK120" t="s" s="2">
         <v>82</v>
@@ -16991,10 +16958,10 @@
         <v>82</v>
       </c>
       <c r="AM120" t="s" s="2">
-        <v>599</v>
+        <v>629</v>
       </c>
       <c r="AN120" t="s" s="2">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="AO120" t="s" s="2">
         <v>82</v>
@@ -17005,10 +16972,10 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -17016,13 +16983,13 @@
       </c>
       <c r="E121" s="2"/>
       <c r="F121" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G121" t="s" s="2">
         <v>81</v>
       </c>
       <c r="H121" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I121" t="s" s="2">
         <v>82</v>
@@ -17031,16 +16998,16 @@
         <v>93</v>
       </c>
       <c r="K121" t="s" s="2">
+        <v>632</v>
+      </c>
+      <c r="L121" t="s" s="2">
+        <v>633</v>
+      </c>
+      <c r="M121" t="s" s="2">
+        <v>634</v>
+      </c>
+      <c r="N121" t="s" s="2">
         <v>635</v>
-      </c>
-      <c r="L121" t="s" s="2">
-        <v>636</v>
-      </c>
-      <c r="M121" t="s" s="2">
-        <v>637</v>
-      </c>
-      <c r="N121" t="s" s="2">
-        <v>638</v>
       </c>
       <c r="O121" s="2"/>
       <c r="P121" t="s" s="2">
@@ -17090,7 +17057,7 @@
         <v>82</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>80</v>
@@ -17111,10 +17078,10 @@
         <v>82</v>
       </c>
       <c r="AM121" t="s" s="2">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="AN121" t="s" s="2">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="AO121" t="s" s="2">
         <v>82</v>
@@ -17125,10 +17092,10 @@
     </row>
     <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -17136,13 +17103,13 @@
       </c>
       <c r="E122" s="2"/>
       <c r="F122" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G122" t="s" s="2">
         <v>81</v>
       </c>
       <c r="H122" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I122" t="s" s="2">
         <v>82</v>
@@ -17151,18 +17118,20 @@
         <v>93</v>
       </c>
       <c r="K122" t="s" s="2">
-        <v>642</v>
+        <v>567</v>
       </c>
       <c r="L122" t="s" s="2">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="M122" t="s" s="2">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="N122" t="s" s="2">
-        <v>645</v>
-      </c>
-      <c r="O122" s="2"/>
+        <v>640</v>
+      </c>
+      <c r="O122" t="s" s="2">
+        <v>641</v>
+      </c>
       <c r="P122" t="s" s="2">
         <v>82</v>
       </c>
@@ -17210,7 +17179,7 @@
         <v>82</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>80</v>
@@ -17222,7 +17191,7 @@
         <v>104</v>
       </c>
       <c r="AJ122" t="s" s="2">
-        <v>170</v>
+        <v>105</v>
       </c>
       <c r="AK122" t="s" s="2">
         <v>82</v>
@@ -17231,10 +17200,10 @@
         <v>82</v>
       </c>
       <c r="AM122" t="s" s="2">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="AN122" t="s" s="2">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="AO122" t="s" s="2">
         <v>82</v>
@@ -17245,10 +17214,10 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -17259,7 +17228,7 @@
         <v>80</v>
       </c>
       <c r="G123" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H123" t="s" s="2">
         <v>82</v>
@@ -17268,23 +17237,19 @@
         <v>82</v>
       </c>
       <c r="J123" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K123" t="s" s="2">
-        <v>577</v>
+        <v>215</v>
       </c>
       <c r="L123" t="s" s="2">
-        <v>648</v>
+        <v>216</v>
       </c>
       <c r="M123" t="s" s="2">
-        <v>649</v>
-      </c>
-      <c r="N123" t="s" s="2">
-        <v>650</v>
-      </c>
-      <c r="O123" t="s" s="2">
-        <v>651</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="N123" s="2"/>
+      <c r="O123" s="2"/>
       <c r="P123" t="s" s="2">
         <v>82</v>
       </c>
@@ -17332,19 +17297,19 @@
         <v>82</v>
       </c>
       <c r="AF123" t="s" s="2">
-        <v>647</v>
+        <v>218</v>
       </c>
       <c r="AG123" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH123" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI123" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AJ123" t="s" s="2">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="AK123" t="s" s="2">
         <v>82</v>
@@ -17353,10 +17318,10 @@
         <v>82</v>
       </c>
       <c r="AM123" t="s" s="2">
-        <v>652</v>
+        <v>82</v>
       </c>
       <c r="AN123" t="s" s="2">
-        <v>653</v>
+        <v>113</v>
       </c>
       <c r="AO123" t="s" s="2">
         <v>82</v>
@@ -17367,21 +17332,21 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
-        <v>82</v>
+        <v>139</v>
       </c>
       <c r="E124" s="2"/>
       <c r="F124" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G124" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H124" t="s" s="2">
         <v>82</v>
@@ -17393,15 +17358,17 @@
         <v>82</v>
       </c>
       <c r="K124" t="s" s="2">
-        <v>215</v>
+        <v>140</v>
       </c>
       <c r="L124" t="s" s="2">
-        <v>216</v>
+        <v>141</v>
       </c>
       <c r="M124" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N124" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="N124" t="s" s="2">
+        <v>143</v>
+      </c>
       <c r="O124" s="2"/>
       <c r="P124" t="s" s="2">
         <v>82</v>
@@ -17438,31 +17405,31 @@
         <v>82</v>
       </c>
       <c r="AB124" t="s" s="2">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AC124" t="s" s="2">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="AD124" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE124" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH124" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI124" t="s" s="2">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AJ124" t="s" s="2">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="AK124" t="s" s="2">
         <v>82</v>
@@ -17474,7 +17441,7 @@
         <v>82</v>
       </c>
       <c r="AN124" t="s" s="2">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="AO124" t="s" s="2">
         <v>82</v>
@@ -17485,14 +17452,14 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
-        <v>139</v>
+        <v>578</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" t="s" s="2">
@@ -17505,24 +17472,26 @@
         <v>82</v>
       </c>
       <c r="I125" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="J125" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K125" t="s" s="2">
         <v>140</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>141</v>
+        <v>579</v>
       </c>
       <c r="M125" t="s" s="2">
-        <v>221</v>
+        <v>580</v>
       </c>
       <c r="N125" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="O125" s="2"/>
+      <c r="O125" t="s" s="2">
+        <v>152</v>
+      </c>
       <c r="P125" t="s" s="2">
         <v>82</v>
       </c>
@@ -17558,19 +17527,19 @@
         <v>82</v>
       </c>
       <c r="AB125" t="s" s="2">
-        <v>144</v>
+        <v>82</v>
       </c>
       <c r="AC125" t="s" s="2">
-        <v>145</v>
+        <v>82</v>
       </c>
       <c r="AD125" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE125" t="s" s="2">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>222</v>
+        <v>581</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>80</v>
@@ -17605,45 +17574,45 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
-        <v>588</v>
+        <v>82</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G126" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H126" t="s" s="2">
         <v>82</v>
       </c>
       <c r="I126" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J126" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K126" t="s" s="2">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>589</v>
+        <v>648</v>
       </c>
       <c r="M126" t="s" s="2">
-        <v>590</v>
+        <v>649</v>
       </c>
       <c r="N126" t="s" s="2">
-        <v>143</v>
+        <v>650</v>
       </c>
       <c r="O126" t="s" s="2">
-        <v>152</v>
+        <v>354</v>
       </c>
       <c r="P126" t="s" s="2">
         <v>82</v>
@@ -17668,13 +17637,13 @@
         <v>82</v>
       </c>
       <c r="X126" t="s" s="2">
-        <v>82</v>
+        <v>355</v>
       </c>
       <c r="Y126" t="s" s="2">
-        <v>82</v>
+        <v>356</v>
       </c>
       <c r="Z126" t="s" s="2">
-        <v>82</v>
+        <v>357</v>
       </c>
       <c r="AA126" t="s" s="2">
         <v>82</v>
@@ -17692,34 +17661,34 @@
         <v>82</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>591</v>
+        <v>647</v>
       </c>
       <c r="AG126" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AH126" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI126" t="s" s="2">
         <v>104</v>
       </c>
       <c r="AJ126" t="s" s="2">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="AK126" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL126" t="s" s="2">
-        <v>82</v>
+        <v>651</v>
       </c>
       <c r="AM126" t="s" s="2">
-        <v>82</v>
+        <v>360</v>
       </c>
       <c r="AN126" t="s" s="2">
-        <v>106</v>
+        <v>361</v>
       </c>
       <c r="AO126" t="s" s="2">
-        <v>82</v>
+        <v>362</v>
       </c>
       <c r="AP126" t="s" s="2">
         <v>82</v>
@@ -17727,10 +17696,10 @@
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -17738,7 +17707,7 @@
       </c>
       <c r="E127" s="2"/>
       <c r="F127" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G127" t="s" s="2">
         <v>92</v>
@@ -17753,19 +17722,19 @@
         <v>93</v>
       </c>
       <c r="K127" t="s" s="2">
-        <v>198</v>
+        <v>433</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="M127" t="s" s="2">
-        <v>659</v>
+        <v>435</v>
       </c>
       <c r="N127" t="s" s="2">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="O127" t="s" s="2">
-        <v>354</v>
+        <v>437</v>
       </c>
       <c r="P127" t="s" s="2">
         <v>82</v>
@@ -17790,13 +17759,13 @@
         <v>82</v>
       </c>
       <c r="X127" t="s" s="2">
-        <v>355</v>
+        <v>82</v>
       </c>
       <c r="Y127" t="s" s="2">
-        <v>356</v>
+        <v>82</v>
       </c>
       <c r="Z127" t="s" s="2">
-        <v>357</v>
+        <v>82</v>
       </c>
       <c r="AA127" t="s" s="2">
         <v>82</v>
@@ -17814,10 +17783,10 @@
         <v>82</v>
       </c>
       <c r="AF127" t="s" s="2">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="AG127" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AH127" t="s" s="2">
         <v>92</v>
@@ -17832,27 +17801,27 @@
         <v>82</v>
       </c>
       <c r="AL127" t="s" s="2">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="AM127" t="s" s="2">
-        <v>360</v>
+        <v>441</v>
       </c>
       <c r="AN127" t="s" s="2">
-        <v>361</v>
+        <v>442</v>
       </c>
       <c r="AO127" t="s" s="2">
-        <v>362</v>
+        <v>82</v>
       </c>
       <c r="AP127" t="s" s="2">
-        <v>82</v>
+        <v>443</v>
       </c>
     </row>
     <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
@@ -17872,22 +17841,22 @@
         <v>82</v>
       </c>
       <c r="J128" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>443</v>
+        <v>198</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>445</v>
+        <v>658</v>
       </c>
       <c r="N128" t="s" s="2">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="O128" t="s" s="2">
-        <v>447</v>
+        <v>503</v>
       </c>
       <c r="P128" t="s" s="2">
         <v>82</v>
@@ -17912,13 +17881,13 @@
         <v>82</v>
       </c>
       <c r="X128" t="s" s="2">
-        <v>82</v>
+        <v>504</v>
       </c>
       <c r="Y128" t="s" s="2">
-        <v>82</v>
+        <v>505</v>
       </c>
       <c r="Z128" t="s" s="2">
-        <v>82</v>
+        <v>506</v>
       </c>
       <c r="AA128" t="s" s="2">
         <v>82</v>
@@ -17936,7 +17905,7 @@
         <v>82</v>
       </c>
       <c r="AF128" t="s" s="2">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="AG128" t="s" s="2">
         <v>80</v>
@@ -17945,7 +17914,7 @@
         <v>92</v>
       </c>
       <c r="AI128" t="s" s="2">
-        <v>104</v>
+        <v>507</v>
       </c>
       <c r="AJ128" t="s" s="2">
         <v>105</v>
@@ -17954,38 +17923,38 @@
         <v>82</v>
       </c>
       <c r="AL128" t="s" s="2">
-        <v>665</v>
+        <v>82</v>
       </c>
       <c r="AM128" t="s" s="2">
-        <v>451</v>
+        <v>106</v>
       </c>
       <c r="AN128" t="s" s="2">
-        <v>452</v>
+        <v>508</v>
       </c>
       <c r="AO128" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP128" t="s" s="2">
-        <v>453</v>
+        <v>82</v>
       </c>
     </row>
     <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
-        <v>82</v>
+        <v>510</v>
       </c>
       <c r="E129" s="2"/>
       <c r="F129" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G129" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H129" t="s" s="2">
         <v>82</v>
@@ -18000,16 +17969,16 @@
         <v>198</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>667</v>
+        <v>511</v>
       </c>
       <c r="M129" t="s" s="2">
-        <v>668</v>
+        <v>512</v>
       </c>
       <c r="N129" t="s" s="2">
-        <v>669</v>
+        <v>513</v>
       </c>
       <c r="O129" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P129" t="s" s="2">
         <v>82</v>
@@ -18034,7 +18003,7 @@
         <v>82</v>
       </c>
       <c r="X129" t="s" s="2">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="Y129" t="s" s="2">
         <v>515</v>
@@ -18058,16 +18027,16 @@
         <v>82</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH129" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI129" t="s" s="2">
-        <v>517</v>
+        <v>104</v>
       </c>
       <c r="AJ129" t="s" s="2">
         <v>105</v>
@@ -18076,31 +18045,31 @@
         <v>82</v>
       </c>
       <c r="AL129" t="s" s="2">
-        <v>82</v>
+        <v>517</v>
       </c>
       <c r="AM129" t="s" s="2">
-        <v>106</v>
+        <v>518</v>
       </c>
       <c r="AN129" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="AO129" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP129" t="s" s="2">
-        <v>82</v>
+        <v>520</v>
       </c>
     </row>
     <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
-        <v>520</v>
+        <v>82</v>
       </c>
       <c r="E130" s="2"/>
       <c r="F130" t="s" s="2">
@@ -18119,19 +18088,19 @@
         <v>82</v>
       </c>
       <c r="K130" t="s" s="2">
-        <v>198</v>
+        <v>83</v>
       </c>
       <c r="L130" t="s" s="2">
-        <v>521</v>
+        <v>662</v>
       </c>
       <c r="M130" t="s" s="2">
-        <v>522</v>
+        <v>663</v>
       </c>
       <c r="N130" t="s" s="2">
-        <v>523</v>
+        <v>570</v>
       </c>
       <c r="O130" t="s" s="2">
-        <v>524</v>
+        <v>571</v>
       </c>
       <c r="P130" t="s" s="2">
         <v>82</v>
@@ -18156,13 +18125,13 @@
         <v>82</v>
       </c>
       <c r="X130" t="s" s="2">
-        <v>514</v>
+        <v>82</v>
       </c>
       <c r="Y130" t="s" s="2">
-        <v>525</v>
+        <v>82</v>
       </c>
       <c r="Z130" t="s" s="2">
-        <v>526</v>
+        <v>82</v>
       </c>
       <c r="AA130" t="s" s="2">
         <v>82</v>
@@ -18180,7 +18149,7 @@
         <v>82</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>80</v>
@@ -18189,154 +18158,32 @@
         <v>81</v>
       </c>
       <c r="AI130" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AJ130" t="s" s="2">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="AK130" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL130" t="s" s="2">
-        <v>527</v>
+        <v>82</v>
       </c>
       <c r="AM130" t="s" s="2">
-        <v>528</v>
+        <v>573</v>
       </c>
       <c r="AN130" t="s" s="2">
-        <v>529</v>
+        <v>574</v>
       </c>
       <c r="AO130" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP130" t="s" s="2">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="131" hidden="true">
-      <c r="A131" t="s" s="2">
-        <v>671</v>
-      </c>
-      <c r="B131" t="s" s="2">
-        <v>671</v>
-      </c>
-      <c r="C131" s="2"/>
-      <c r="D131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="E131" s="2"/>
-      <c r="F131" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G131" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="H131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="I131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="J131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="K131" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="L131" t="s" s="2">
-        <v>672</v>
-      </c>
-      <c r="M131" t="s" s="2">
-        <v>673</v>
-      </c>
-      <c r="N131" t="s" s="2">
-        <v>580</v>
-      </c>
-      <c r="O131" t="s" s="2">
-        <v>581</v>
-      </c>
-      <c r="P131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Q131" s="2"/>
-      <c r="R131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="S131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Y131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Z131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AA131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AB131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AD131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AE131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF131" t="s" s="2">
-        <v>671</v>
-      </c>
-      <c r="AG131" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH131" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AJ131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AK131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AM131" t="s" s="2">
-        <v>583</v>
-      </c>
-      <c r="AN131" t="s" s="2">
-        <v>584</v>
-      </c>
-      <c r="AO131" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP131" t="s" s="2">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP131">
+  <autoFilter ref="A1:AP130">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -18346,7 +18193,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI130">
+  <conditionalFormatting sqref="A2:AI129">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changes in Category.Slicing & CodeValues
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-age.xlsx
+++ b/output/StructureDefinition-cde-age.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-10T10:38:26+01:00</t>
+    <t>2023-03-13T12:04:54+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1157,7 +1157,7 @@
     <t>Observation.code.coding.system</t>
   </si>
   <si>
-    <t>http://loinc.org</t>
+    <t>https://fhir.loinc.org</t>
   </si>
   <si>
     <t>Observation.code.coding.version</t>
@@ -1181,7 +1181,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient)
+    <t xml:space="preserve">Reference(Patient|Group|Device|Location)
 </t>
   </si>
   <si>
@@ -1537,7 +1537,7 @@
     <t>Observation.value[x].code</t>
   </si>
   <si>
-    <t>Coded responses from the common UCUM units for length.</t>
+    <t>Coded responses from the common UCUM units for number concentration.</t>
   </si>
   <si>
     <t>The preferred system is UCUM, but SNOMED CT can also be used (for customary units) or ISO 4217 for currency.  The context of use may additionally require a code from a particular system.</t>
@@ -1549,7 +1549,7 @@
     <t>wk | a</t>
   </si>
   <si>
-    <t>http://somewhere.org/fhir/uv/myig/ValueSet/vs-mass-concentration-units</t>
+    <t>http://somewhere.org/fhir/uv/myig/ValueSet/vs-time-units</t>
   </si>
   <si>
     <t>Quantity.code</t>
@@ -1980,7 +1980,7 @@
     <t>Observation.derivedFrom</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(DocumentReference|QuestionnaireResponse|Observation)
+    <t xml:space="preserve">Reference(DocumentReference|ImagingStudy|Media|QuestionnaireResponse|Observation|MolecularSequence)
 </t>
   </si>
   <si>
@@ -2430,7 +2430,7 @@
     <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="60.51953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="68.2421875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="54.5859375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="88.40625" customWidth="true" bestFit="true"/>
@@ -4223,7 +4223,7 @@
         <v>206</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="AE15" t="s" s="2">
         <v>207</v>
@@ -12985,13 +12985,13 @@
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G88" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H88" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I88" t="s" s="2">
         <v>82</v>
@@ -16983,13 +16983,13 @@
       </c>
       <c r="E121" s="2"/>
       <c r="F121" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G121" t="s" s="2">
         <v>81</v>
       </c>
       <c r="H121" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I121" t="s" s="2">
         <v>82</v>

</xml_diff>